<commit_message>
Fixing fuel emission factors
</commit_message>
<xml_diff>
--- a/src_files/data_files/fueldata_maf2020.xlsx
+++ b/src_files/data_files/fueldata_maf2020.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C5FF66-A1C9-45BE-8571-20CDB0E6DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91074A5D-8600-4C66-A35A-B5CBF1AC5B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fueldata" sheetId="1" r:id="rId1"/>
+    <sheet name="data_fuelEmissions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Bottom">OFFSET(#REF!,1,0,COUNT(#REF!),1)</definedName>
     <definedName name="Labels">OFFSET(Bottom,0,-1)</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="21">
   <si>
     <t>Scenario</t>
   </si>
@@ -69,12 +70,6 @@
     <t>MSW</t>
   </si>
   <si>
-    <t>DRservice1</t>
-  </si>
-  <si>
-    <t>DRservice0</t>
-  </si>
-  <si>
     <t>Hydrogencommod</t>
   </si>
   <si>
@@ -102,10 +97,13 @@
     <t>Black liquor</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>grid</t>
+  </si>
+  <si>
+    <t>tCO2/TJ</t>
+  </si>
+  <si>
+    <t>tCO2/MWh</t>
   </si>
 </sst>
 </file>
@@ -304,10 +302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -326,13 +324,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
@@ -343,13 +341,14 @@
         <v>2025</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6">
         <v>27</v>
       </c>
       <c r="E2" s="7">
-        <v>94</v>
+        <f>IFERROR(VLOOKUP($C2, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -366,6 +365,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="7">
+        <f>IFERROR(VLOOKUP($C3, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -383,7 +383,8 @@
         <v>55</v>
       </c>
       <c r="E4" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C4, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -394,13 +395,14 @@
         <v>2025</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="6">
         <v>46</v>
       </c>
       <c r="E5" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C5, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.28079999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -411,13 +413,14 @@
         <v>2025</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="6">
         <v>65</v>
       </c>
       <c r="E6" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C6, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.25559999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -434,7 +437,8 @@
         <v>8</v>
       </c>
       <c r="E7" s="7">
-        <v>101</v>
+        <f>IFERROR(VLOOKUP($C7, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.37080000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -451,6 +455,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="7">
+        <f>IFERROR(VLOOKUP($C8, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -462,12 +467,13 @@
         <v>2025</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7">
+        <f>IFERROR(VLOOKUP($C9, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -485,7 +491,8 @@
         <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C10, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -496,324 +503,343 @@
         <v>2025</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="7">
         <v>10</v>
       </c>
       <c r="E11" s="7">
-        <v>100</v>
+        <f>IFERROR(VLOOKUP($C11, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>2025</v>
-      </c>
-      <c r="C12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>20</v>
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2040</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="6">
+        <v>35</v>
+      </c>
+      <c r="E12" s="7">
+        <f>IFERROR(VLOOKUP($C12, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>2025</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>20</v>
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2040</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="E13" s="7">
+        <f>IFERROR(VLOOKUP($C13, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="3">
         <v>2040</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D14" s="6">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="E14" s="7">
-        <v>94</v>
+        <f>IFERROR(VLOOKUP($C14, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="3">
         <v>2040</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D15" s="6">
-        <v>2.5</v>
+        <v>65</v>
       </c>
       <c r="E15" s="7">
-        <v>0</v>
+        <f>IFERROR(VLOOKUP($C15, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.28079999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B16" s="3">
         <v>2040</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E16" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C16, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.25559999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B17" s="3">
         <v>2040</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="D17" s="6">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="E17" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C17, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.37080000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3">
         <v>2040</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D18" s="6">
-        <v>90</v>
+        <v>28</v>
       </c>
       <c r="E18" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C18, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B19" s="3">
         <v>2040</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E19" s="7">
-        <v>101</v>
+        <f>IFERROR(VLOOKUP($C19, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="3">
         <v>2040</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" s="6">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E20" s="7">
-        <v>0</v>
+        <f>IFERROR(VLOOKUP($C20, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21" s="3">
         <v>2040</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
+      <c r="C21" t="s">
+        <v>16</v>
       </c>
       <c r="D21" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E21" s="7">
-        <v>0</v>
+        <f>IFERROR(VLOOKUP($C21, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="3">
         <v>2040</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="6">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="D22" s="7">
+        <v>70</v>
       </c>
       <c r="E22" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C22, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B23" s="3">
-        <v>2040</v>
-      </c>
-      <c r="C23" t="s">
-        <v>18</v>
+        <v>2030</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D23" s="6">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="E23" s="7">
-        <v>100</v>
+        <f>IFERROR(VLOOKUP($C23, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B24" s="3">
-        <v>2040</v>
-      </c>
-      <c r="C24" t="s">
-        <v>9</v>
+        <v>2030</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="D24" s="6">
-        <v>0</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>20</v>
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="7">
+        <f>IFERROR(VLOOKUP($C24, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B25" s="3">
-        <v>2040</v>
-      </c>
-      <c r="C25" t="s">
-        <v>10</v>
+        <v>2030</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>20</v>
+        <v>55</v>
+      </c>
+      <c r="E25" s="7">
+        <f>IFERROR(VLOOKUP($C25, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.19800000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26" s="3">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="7">
-        <v>70</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
+      </c>
+      <c r="D26" s="6">
+        <v>65</v>
+      </c>
+      <c r="E26" s="7">
+        <f>IFERROR(VLOOKUP($C26, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.28079999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27" s="3">
         <v>2030</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="6">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="E27" s="7">
-        <v>94</v>
+        <f>IFERROR(VLOOKUP($C27, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.25559999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" s="3">
         <v>2030</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D28" s="6">
-        <v>2.5</v>
+        <v>9</v>
       </c>
       <c r="E28" s="7">
-        <v>0</v>
+        <f>IFERROR(VLOOKUP($C28, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.37080000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29" s="3">
         <v>2030</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D29" s="6">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="E29" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C29, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30" s="3">
         <v>2030</v>
@@ -822,350 +848,245 @@
         <v>17</v>
       </c>
       <c r="D30" s="6">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="E30" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C30, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31" s="3">
         <v>2030</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D31" s="6">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E31" s="7">
-        <v>78</v>
+        <f>IFERROR(VLOOKUP($C31, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32" s="3">
         <v>2030</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>6</v>
+      <c r="C32" t="s">
+        <v>16</v>
       </c>
       <c r="D32" s="6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E32" s="7">
-        <v>101</v>
+        <f>IFERROR(VLOOKUP($C32, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.41399999999999998</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33" s="3">
         <v>2030</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="6">
-        <v>28</v>
+        <v>9</v>
+      </c>
+      <c r="D33" s="7">
+        <v>75</v>
       </c>
       <c r="E33" s="7">
+        <f>IFERROR(VLOOKUP($C33, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="3">
-        <v>2030</v>
+      <c r="A34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34">
+        <v>2035</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="6">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D34" s="7">
+        <v>27</v>
       </c>
       <c r="E34" s="7">
-        <v>0</v>
+        <f>IFERROR(VLOOKUP($C34, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.34200000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="3">
-        <v>2030</v>
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35">
+        <v>2035</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="7">
+        <v>2.5</v>
+      </c>
+      <c r="E35" s="7">
+        <f>IFERROR(VLOOKUP($C35, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>2035</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="7">
+        <v>55</v>
+      </c>
+      <c r="E36" s="7">
+        <f>IFERROR(VLOOKUP($C36, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>2035</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="7">
+        <v>46</v>
+      </c>
+      <c r="E37" s="7">
+        <f>IFERROR(VLOOKUP($C37, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.28079999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38">
+        <v>2035</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="7">
+        <v>65</v>
+      </c>
+      <c r="E38" s="7">
+        <f>IFERROR(VLOOKUP($C38, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.25559999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39">
+        <v>2035</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="8">
         <v>8</v>
       </c>
-      <c r="D35" s="6">
-        <v>1</v>
-      </c>
-      <c r="E35" s="7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="3">
-        <v>2030</v>
-      </c>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="6">
-        <v>10</v>
-      </c>
-      <c r="E36" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="3">
-        <v>2030</v>
-      </c>
-      <c r="C37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="6">
-        <v>0</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="3">
-        <v>2030</v>
-      </c>
-      <c r="C38" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="6">
-        <v>0</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="3">
-        <v>2030</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="7">
-        <v>75</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>20</v>
+      <c r="E39" s="7">
+        <f>IFERROR(VLOOKUP($C39, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.37080000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>2035</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D40" s="7">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E40" s="7">
-        <v>94</v>
+        <f>IFERROR(VLOOKUP($C40, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>2035</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D41" s="7">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E41" s="7">
+        <f>IFERROR(VLOOKUP($C41, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>2035</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D42" s="7">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="E42" s="7">
-        <v>57</v>
+        <f>IFERROR(VLOOKUP($C42, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.14399999999999999</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>2035</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>17</v>
+      <c r="C43" t="s">
+        <v>16</v>
       </c>
       <c r="D43" s="7">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E43" s="7">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44">
-        <v>2035</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D44" s="7">
-        <v>65</v>
-      </c>
-      <c r="E44" s="7">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45">
-        <v>2035</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="8">
-        <v>8</v>
-      </c>
-      <c r="E45" s="7">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46">
-        <v>2035</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="7">
-        <v>26</v>
-      </c>
-      <c r="E46" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47">
-        <v>2035</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="7">
-        <v>1</v>
-      </c>
-      <c r="E47" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48">
-        <v>2035</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D48" s="7">
-        <v>10</v>
-      </c>
-      <c r="E48" s="7">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>2035</v>
-      </c>
-      <c r="C49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D49" s="7">
-        <v>0</v>
-      </c>
-      <c r="E49" s="7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50">
-        <v>2035</v>
-      </c>
-      <c r="C50" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>20</v>
+        <f>IFERROR(VLOOKUP($C43, data_fuelEmissions!$D$4:$F$14,3,FALSE), 0)</f>
+        <v>0.41399999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1176,4 +1097,147 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F8F8B4-D0EB-4745-A354-04E35BFEA174}">
+  <dimension ref="D4:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>95</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F6" si="0">E5*3.6/1000</f>
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>55</v>
+      </c>
+      <c r="F7">
+        <f>E7*3.6/1000</f>
+        <v>0.19800000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>78</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F14" si="1">E8*3.6/1000</f>
+        <v>0.28079999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>71</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.25559999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>103</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.37080000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>115</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>